<commit_message>
ex07 p1 plus docu
</commit_message>
<xml_diff>
--- a/ex07/ex07.xlsx
+++ b/ex07/ex07.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CSE\CSMC\CSMC_2021WS\ex07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922FA903-FA89-4E69-86C1-75E43A1F946D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99770B71-4CC0-41B4-A571-8A8EF8F865F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>vector size</t>
   </si>
@@ -45,16 +54,28 @@
     <t>128x128</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2nd_kernel_on_cpu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2nd_kernel_on_gpu</t>
-  </si>
-  <si>
     <t>256x256</t>
   </si>
   <si>
     <t>512x512</t>
+  </si>
+  <si>
+    <t>(N+255)/256x256</t>
+  </si>
+  <si>
+    <t>Block_size</t>
+  </si>
+  <si>
+    <t>no atomicAdd() - final sum on CPU</t>
+  </si>
+  <si>
+    <t>no atomicAdd() - final sum on GPU</t>
+  </si>
+  <si>
+    <t>one atomicAdd() per workgroup</t>
+  </si>
+  <si>
+    <t>one atomicAdd() per warp</t>
   </si>
 </sst>
 </file>
@@ -95,12 +116,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,7 +181,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> 2nd_kernel_on_cpu</c:v>
+                  <c:v>no atomicAdd() - final sum on CPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -275,7 +299,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> 2nd_kernel_on_gpu</c:v>
+                  <c:v>no atomicAdd() - final sum on GPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -393,7 +417,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> atomic_add_per_workgroup</c:v>
+                  <c:v>one atomicAdd() per workgroup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -511,7 +535,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> atomic_add_per_warp</c:v>
+                  <c:v>one atomicAdd() per warp</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -885,7 +909,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.17518310442741022"/>
           <c:y val="5.4397054534849811E-2"/>
-          <c:w val="0.4663337244667905"/>
+          <c:w val="0.54648271497687151"/>
           <c:h val="0.35763998250218726"/>
         </c:manualLayout>
       </c:layout>
@@ -1001,7 +1025,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> 2nd_kernel_on_cpu</c:v>
+                  <c:v>no atomicAdd() - final sum on CPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1118,7 +1142,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> 2nd_kernel_on_gpu</c:v>
+                  <c:v>no atomicAdd() - final sum on GPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1235,7 +1259,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> atomic_add_per_workgroup</c:v>
+                  <c:v>one atomicAdd() per workgroup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1352,7 +1376,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> atomic_add_per_warp</c:v>
+                  <c:v>one atomicAdd() per warp</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1725,7 +1749,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.17518310442741022"/>
           <c:y val="5.4397054534849811E-2"/>
-          <c:w val="0.4663337244667905"/>
+          <c:w val="0.5492464732703225"/>
           <c:h val="0.35763998250218726"/>
         </c:manualLayout>
       </c:layout>
@@ -1841,7 +1865,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> 2nd_kernel_on_cpu</c:v>
+                  <c:v>no atomicAdd() - final sum on CPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1958,7 +1982,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> 2nd_kernel_on_gpu</c:v>
+                  <c:v>no atomicAdd() - final sum on GPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2075,7 +2099,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> atomic_add_per_workgroup</c:v>
+                  <c:v>one atomicAdd() per workgroup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2192,7 +2216,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> atomic_add_per_warp</c:v>
+                  <c:v>one atomicAdd() per warp</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2566,7 +2590,848 @@
           <c:yMode val="edge"/>
           <c:x val="0.17518310442741022"/>
           <c:y val="5.4397054534849811E-2"/>
-          <c:w val="0.4663337244667905"/>
+          <c:w val="0.52437264862926292"/>
+          <c:h val="0.35763998250218726"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1758696916255077"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.7594237629243783"/>
+          <c:h val="0.77475211431904345"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>no atomicAdd() - final sum on CPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$47:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$47:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.6E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8999999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3999999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.06E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>2.42E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>7.27E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>2.075E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>6.8440000000000003E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D0F1-43E3-BC62-49F960B6D3C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>no atomicAdd() - final sum on GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$47:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$47:$C$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5.5000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.4999999999999994E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.2999999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>2.4000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>7.0600000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>2.029E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>6.646E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D0F1-43E3-BC62-49F960B6D3C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>one atomicAdd() per workgroup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$47:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$D$47:$D$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.3999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8999999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.02E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>2.3499999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>7.0399999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>2.0249999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>6.6410000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D0F1-43E3-BC62-49F960B6D3C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>one atomicAdd() per warp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$47:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$E$47:$E$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4999999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3999999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6000000000000003E-5</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>1.8900000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>5.4500000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>1.549E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>5.0639999999999999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D0F1-43E3-BC62-49F960B6D3C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="943932975"/>
+        <c:axId val="1346020255"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="943932975"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100"/>
+                  <a:t>vector size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1346020255"/>
+        <c:crossesAt val="1.0000000000000004E-5"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1346020255"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0000000000000002E-2"/>
+          <c:min val="1.0000000000000004E-5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100"/>
+                  <a:t>execution time in s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="943932975"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17518310442741022"/>
+          <c:y val="5.4397054534849811E-2"/>
+          <c:w val="0.5575377481506758"/>
           <c:h val="0.35763998250218726"/>
         </c:manualLayout>
       </c:layout>
@@ -2763,6 +3628,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3796,6 +4701,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4351,16 +5772,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>107673</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>124238</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>8283</xdr:rowOff>
+      <xdr:rowOff>165653</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>412474</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>84483</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>429039</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>51353</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4420,6 +5841,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B636D2D-CF02-4258-820F-FE7AC19BB089}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4691,10 +6150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E37"/>
+  <dimension ref="A2:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4709,16 +6168,16 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4876,7 +6335,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -5051,7 +6510,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -5139,7 +6598,7 @@
         <v>1.55E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>100000</v>
       </c>
@@ -5156,7 +6615,7 @@
         <v>1.6000000000000001E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>300000</v>
       </c>
@@ -5173,7 +6632,7 @@
         <v>1.7699999999999999E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>1000000</v>
       </c>
@@ -5190,7 +6649,7 @@
         <v>2.5900000000000001E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>3000000</v>
       </c>
@@ -5207,7 +6666,7 @@
         <v>4.75E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>10000000</v>
       </c>
@@ -5222,6 +6681,220 @@
       </c>
       <c r="E37">
         <v>1.1770000000000001E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B47" s="3">
+        <v>4.6E-5</v>
+      </c>
+      <c r="C47" s="2">
+        <v>5.5000000000000002E-5</v>
+      </c>
+      <c r="D47" s="2">
+        <v>4.3999999999999999E-5</v>
+      </c>
+      <c r="E47" s="2">
+        <v>3.4E-5</v>
+      </c>
+      <c r="F47">
+        <f t="shared" ref="F47:F55" si="0">_xlfn.CEILING.MATH((A47+255)/256)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="1">
+        <v>3000</v>
+      </c>
+      <c r="B48" s="3">
+        <v>4.6E-5</v>
+      </c>
+      <c r="C48" s="2">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="D48" s="2">
+        <v>4.3999999999999999E-5</v>
+      </c>
+      <c r="E48" s="2">
+        <v>3.4999999999999997E-5</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B49" s="3">
+        <v>4.8999999999999998E-5</v>
+      </c>
+      <c r="C49" s="2">
+        <v>6.4999999999999994E-5</v>
+      </c>
+      <c r="D49" s="2">
+        <v>4.6E-5</v>
+      </c>
+      <c r="E49" s="2">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B50" s="3">
+        <v>6.3999999999999997E-5</v>
+      </c>
+      <c r="C50" s="2">
+        <v>7.7999999999999999E-5</v>
+      </c>
+      <c r="D50" s="2">
+        <v>5.8999999999999998E-5</v>
+      </c>
+      <c r="E50" s="2">
+        <v>5.3999999999999998E-5</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1.06E-4</v>
+      </c>
+      <c r="C51">
+        <v>1.2999999999999999E-4</v>
+      </c>
+      <c r="D51">
+        <v>1.02E-4</v>
+      </c>
+      <c r="E51" s="2">
+        <v>8.6000000000000003E-5</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="1">
+        <v>300000</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2.42E-4</v>
+      </c>
+      <c r="C52">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="D52">
+        <v>2.3499999999999999E-4</v>
+      </c>
+      <c r="E52">
+        <v>1.8900000000000001E-4</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="B53" s="1">
+        <v>7.27E-4</v>
+      </c>
+      <c r="C53">
+        <v>7.0600000000000003E-4</v>
+      </c>
+      <c r="D53">
+        <v>7.0399999999999998E-4</v>
+      </c>
+      <c r="E53">
+        <v>5.4500000000000002E-4</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>3908</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="1">
+        <v>3000000</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2.075E-3</v>
+      </c>
+      <c r="C54">
+        <v>2.029E-3</v>
+      </c>
+      <c r="D54">
+        <v>2.0249999999999999E-3</v>
+      </c>
+      <c r="E54">
+        <v>1.549E-3</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>11720</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="B55" s="1">
+        <v>6.8440000000000003E-3</v>
+      </c>
+      <c r="C55">
+        <v>6.646E-3</v>
+      </c>
+      <c r="D55">
+        <v>6.6410000000000002E-3</v>
+      </c>
+      <c r="E55">
+        <v>5.0639999999999999E-3</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>39064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ex07 p2 docu done. part 2.3 missing
</commit_message>
<xml_diff>
--- a/ex07/ex07.xlsx
+++ b/ex07/ex07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CSE\CSMC\CSMC_2021WS\ex07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B774B1-FB35-47FC-A6FC-BF91F9E4F79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F2B90A-7B9F-43DC-B814-8F0EE5028131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,13 +82,13 @@
     <t xml:space="preserve"> execution time</t>
   </si>
   <si>
-    <t>openCL on GPU</t>
+    <t>OpenCL on GPU</t>
   </si>
   <si>
-    <t>cuda on GPU</t>
+    <t>CUDA on GPU</t>
   </si>
   <si>
-    <t>openCL on CPU</t>
+    <t>OpenCL on CPU</t>
   </si>
 </sst>
 </file>
@@ -3560,7 +3560,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>openCL on GPU</c:v>
+                  <c:v>OpenCL on GPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3677,7 +3677,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>cuda on GPU</c:v>
+                  <c:v>CUDA on GPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3794,7 +3794,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>openCL on CPU</c:v>
+                  <c:v>OpenCL on CPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8241,8 +8241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680D2880-9682-4113-92A8-D218BA9FFD8B}">
   <dimension ref="A4:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8275,6 +8275,7 @@
       <c r="D5" s="2">
         <v>1.323E-3</v>
       </c>
+      <c r="E5" s="2"/>
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
     </row>
@@ -8291,6 +8292,7 @@
       <c r="D6" s="2">
         <v>1.4139999999999999E-3</v>
       </c>
+      <c r="E6" s="2"/>
       <c r="G6" s="1"/>
       <c r="H6" s="2"/>
     </row>
@@ -8307,6 +8309,7 @@
       <c r="D7" s="2">
         <v>1.127E-3</v>
       </c>
+      <c r="E7" s="2"/>
       <c r="G7" s="1"/>
       <c r="H7" s="2"/>
     </row>
@@ -8323,6 +8326,7 @@
       <c r="D8" s="2">
         <v>1.3450000000000001E-3</v>
       </c>
+      <c r="E8" s="2"/>
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
     </row>
@@ -8339,6 +8343,7 @@
       <c r="D9" s="2">
         <v>1.1919999999999999E-3</v>
       </c>
+      <c r="E9" s="2"/>
       <c r="G9" s="1"/>
       <c r="H9" s="2"/>
     </row>
@@ -8355,6 +8360,7 @@
       <c r="D10" s="2">
         <v>2.9039999999999999E-3</v>
       </c>
+      <c r="E10" s="2"/>
       <c r="G10" s="1"/>
       <c r="H10" s="2"/>
     </row>
@@ -8371,6 +8377,7 @@
       <c r="D11" s="2">
         <v>5.6080000000000001E-3</v>
       </c>
+      <c r="E11" s="2"/>
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
     </row>
@@ -8387,6 +8394,7 @@
       <c r="D12" s="2">
         <v>1.2241999999999999E-2</v>
       </c>
+      <c r="E12" s="2"/>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
     </row>
@@ -8403,6 +8411,7 @@
       <c r="D13" s="2">
         <v>7.1274000000000004E-2</v>
       </c>
+      <c r="E13" s="2"/>
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
     </row>

</xml_diff>

<commit_message>
ex07 - p3 - matvec runs single threaded, some corrections in p2
</commit_message>
<xml_diff>
--- a/ex07/ex07.xlsx
+++ b/ex07/ex07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CSE\CSMC\CSMC_2021WS\ex07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F2B90A-7B9F-43DC-B814-8F0EE5028131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C151EE8E-5055-49AF-AD9A-2E030D0F635D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>vector size</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>OpenCL on CPU</t>
+  </si>
+  <si>
+    <t>rel CPU/GPU</t>
   </si>
 </sst>
 </file>
@@ -3632,31 +3635,31 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2.4000000000000001E-5</c:v>
+                  <c:v>3.8000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4000000000000001E-5</c:v>
+                  <c:v>3.8999999999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6999999999999999E-5</c:v>
+                  <c:v>4.0000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5000000000000001E-5</c:v>
+                  <c:v>4.6E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5999999999999998E-5</c:v>
+                  <c:v>3.8999999999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6999999999999998E-5</c:v>
+                  <c:v>5.1999999999999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.5000000000000006E-5</c:v>
+                  <c:v>1.06E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.63E-4</c:v>
+                  <c:v>1.7699999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.8000000000000001E-4</c:v>
+                  <c:v>4.9899999999999999E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3866,31 +3869,31 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.323E-3</c:v>
+                  <c:v>3.9300000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4139999999999999E-3</c:v>
+                  <c:v>3.9399999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.127E-3</c:v>
+                  <c:v>4.15E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3450000000000001E-3</c:v>
+                  <c:v>4.8500000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1919999999999999E-3</c:v>
+                  <c:v>4.4900000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.9039999999999999E-3</c:v>
+                  <c:v>4.9700000000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.6080000000000001E-3</c:v>
+                  <c:v>1.9940000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2241999999999999E-2</c:v>
+                  <c:v>6.8040000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.1274000000000004E-2</c:v>
+                  <c:v>7.2691000000000006E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4165,10 +4168,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18809098862642171"/>
-          <c:y val="8.3911490230387867E-2"/>
-          <c:w val="0.32104024496937883"/>
-          <c:h val="0.24942184310294546"/>
+          <c:x val="0.17977680354216358"/>
+          <c:y val="5.6133712452610104E-2"/>
+          <c:w val="0.32968416871976269"/>
+          <c:h val="0.27451698745990083"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -7184,15 +7187,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:colOff>321879</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>85889</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:colOff>17079</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>162089</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8242,7 +8245,7 @@
   <dimension ref="A4:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8260,6 +8263,9 @@
       <c r="D4" t="s">
         <v>17</v>
       </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:8">
@@ -8267,15 +8273,18 @@
         <v>1000</v>
       </c>
       <c r="B5" s="2">
-        <v>2.4000000000000001E-5</v>
+        <v>3.8000000000000002E-5</v>
       </c>
       <c r="C5" s="2">
         <v>3.8999999999999999E-5</v>
       </c>
       <c r="D5" s="2">
-        <v>1.323E-3</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>3.9300000000000001E-4</v>
+      </c>
+      <c r="E5" s="2">
+        <f>D5/B5</f>
+        <v>10.342105263157894</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
     </row>
@@ -8284,15 +8293,18 @@
         <v>3000</v>
       </c>
       <c r="B6" s="2">
-        <v>2.4000000000000001E-5</v>
+        <v>3.8999999999999999E-5</v>
       </c>
       <c r="C6" s="2">
         <v>4.1E-5</v>
       </c>
       <c r="D6" s="2">
-        <v>1.4139999999999999E-3</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" ref="E6:E13" si="0">D6/B6</f>
+        <v>10.102564102564102</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="2"/>
     </row>
@@ -8301,15 +8313,18 @@
         <v>10000</v>
       </c>
       <c r="B7" s="2">
-        <v>2.6999999999999999E-5</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="C7" s="2">
         <v>3.6999999999999998E-5</v>
       </c>
       <c r="D7" s="2">
-        <v>1.127E-3</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>4.15E-4</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>10.375</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="2"/>
     </row>
@@ -8318,15 +8333,18 @@
         <v>30000</v>
       </c>
       <c r="B8" s="2">
-        <v>2.5000000000000001E-5</v>
+        <v>4.6E-5</v>
       </c>
       <c r="C8" s="2">
         <v>3.8999999999999999E-5</v>
       </c>
       <c r="D8" s="2">
-        <v>1.3450000000000001E-3</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>4.8500000000000003E-4</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>10.543478260869566</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
     </row>
@@ -8335,15 +8353,18 @@
         <v>100000</v>
       </c>
       <c r="B9" s="2">
-        <v>2.5999999999999998E-5</v>
+        <v>3.8999999999999999E-5</v>
       </c>
       <c r="C9" s="2">
         <v>4.1999999999999998E-5</v>
       </c>
       <c r="D9" s="2">
-        <v>1.1919999999999999E-3</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>4.4900000000000002E-4</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>11.512820512820513</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="2"/>
     </row>
@@ -8352,15 +8373,18 @@
         <v>300000</v>
       </c>
       <c r="B10" s="2">
-        <v>3.6999999999999998E-5</v>
+        <v>5.1999999999999997E-5</v>
       </c>
       <c r="C10" s="2">
         <v>5.1E-5</v>
       </c>
       <c r="D10" s="2">
-        <v>2.9039999999999999E-3</v>
-      </c>
-      <c r="E10" s="2"/>
+        <v>4.9700000000000005E-4</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>9.5576923076923084</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="2"/>
     </row>
@@ -8369,15 +8393,18 @@
         <v>1000000</v>
       </c>
       <c r="B11" s="2">
-        <v>8.5000000000000006E-5</v>
+        <v>1.06E-4</v>
       </c>
       <c r="C11" s="2">
         <v>8.2000000000000001E-5</v>
       </c>
       <c r="D11" s="2">
-        <v>5.6080000000000001E-3</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>1.9940000000000001E-3</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>18.811320754716981</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
     </row>
@@ -8386,15 +8413,18 @@
         <v>3000000</v>
       </c>
       <c r="B12" s="2">
-        <v>1.63E-4</v>
+        <v>1.7699999999999999E-4</v>
       </c>
       <c r="C12">
         <v>1.7100000000000001E-4</v>
       </c>
       <c r="D12" s="2">
-        <v>1.2241999999999999E-2</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>6.8040000000000002E-3</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>38.440677966101696</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
     </row>
@@ -8403,15 +8433,18 @@
         <v>10000000</v>
       </c>
       <c r="B13" s="2">
-        <v>4.8000000000000001E-4</v>
+        <v>4.9899999999999999E-4</v>
       </c>
       <c r="C13">
         <v>4.9200000000000003E-4</v>
       </c>
       <c r="D13" s="2">
-        <v>7.1274000000000004E-2</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>7.2691000000000006E-2</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>145.67334669338678</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
     </row>
@@ -8421,25 +8454,33 @@
     <row r="16" spans="1:8">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:7">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:7">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:7">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:7">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:7">
       <c r="A21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:7">
       <c r="A22" s="1"/>
+      <c r="F22" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G22" s="2">
+        <v>3.9300000000000001E-4</v>
+      </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:7">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>0</v>
@@ -8447,8 +8488,14 @@
       <c r="C23" t="s">
         <v>14</v>
       </c>
+      <c r="F23" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G23" s="2">
+        <v>3.9399999999999998E-4</v>
+      </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:7">
       <c r="A24" s="1"/>
       <c r="B24" s="1">
         <v>1000</v>
@@ -8456,56 +8503,98 @@
       <c r="C24" s="2">
         <v>1.323E-3</v>
       </c>
+      <c r="F24" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G24" s="2">
+        <v>4.15E-4</v>
+      </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:7">
       <c r="B25" s="1">
         <v>3000</v>
       </c>
       <c r="C25" s="2">
         <v>1.4139999999999999E-3</v>
       </c>
+      <c r="F25" s="1">
+        <v>30000</v>
+      </c>
+      <c r="G25" s="2">
+        <v>4.8500000000000003E-4</v>
+      </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:7">
       <c r="B26" s="1">
         <v>10000</v>
       </c>
       <c r="C26" s="2">
         <v>1.127E-3</v>
       </c>
+      <c r="F26" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G26" s="2">
+        <v>4.4900000000000002E-4</v>
+      </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:7">
       <c r="B27" s="1">
         <v>30000</v>
       </c>
       <c r="C27" s="2">
         <v>1.3450000000000001E-3</v>
       </c>
+      <c r="F27" s="1">
+        <v>300000</v>
+      </c>
+      <c r="G27" s="2">
+        <v>4.9700000000000005E-4</v>
+      </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:7">
       <c r="B28" s="1">
         <v>100000</v>
       </c>
       <c r="C28" s="2">
         <v>1.1919999999999999E-3</v>
       </c>
+      <c r="F28" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1.9940000000000001E-3</v>
+      </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:7">
       <c r="B29" s="1">
         <v>300000</v>
       </c>
       <c r="C29" s="2">
         <v>2.9039999999999999E-3</v>
       </c>
+      <c r="F29" s="1">
+        <v>3000000</v>
+      </c>
+      <c r="G29" s="2">
+        <v>6.8040000000000002E-3</v>
+      </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:7">
       <c r="B30" s="1">
         <v>1000000</v>
       </c>
       <c r="C30" s="2">
         <v>5.6080000000000001E-3</v>
       </c>
+      <c r="F30" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="G30" s="2">
+        <v>7.2691000000000006E-2</v>
+      </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:7">
       <c r="B31" s="1">
         <v>3000000</v>
       </c>
@@ -8513,7 +8602,7 @@
         <v>1.2241999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:7">
       <c r="B32" s="1">
         <v>10000000</v>
       </c>

</xml_diff>

<commit_message>
ex07 p3 - both kernels work - time to get benchmarking
</commit_message>
<xml_diff>
--- a/ex07/ex07.xlsx
+++ b/ex07/ex07.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CSE\CSMC\CSMC_2021WS\ex07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C151EE8E-5055-49AF-AD9A-2E030D0F635D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F39C6A-C95B-4F62-965F-D6F79A502C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1" sheetId="1" r:id="rId1"/>
     <sheet name="P2" sheetId="2" r:id="rId2"/>
+    <sheet name="P3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -8244,7 +8245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680D2880-9682-4113-92A8-D218BA9FFD8B}">
   <dimension ref="A4:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -8615,4 +8616,69 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC7C974-8D29-467D-B540-E901A50BF91D}">
+  <dimension ref="A3:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <f>A3*2</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <f t="shared" ref="A5:A19" si="0">A4*2</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>3840</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ex07 - p3 - benchmarks done
</commit_message>
<xml_diff>
--- a/ex07/ex07.xlsx
+++ b/ex07/ex07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CSE\CSMC\CSMC_2021WS\ex07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F39C6A-C95B-4F62-965F-D6F79A502C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2949B0D1-61BE-447B-BEC5-DBF1B054F881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>vector size</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>rel CPU/GPU</t>
+  </si>
+  <si>
+    <t>few nonzeros</t>
+  </si>
+  <si>
+    <t>many nonzeros</t>
+  </si>
+  <si>
+    <t>one thread per row</t>
+  </si>
+  <si>
+    <t>one group per row</t>
   </si>
 </sst>
 </file>
@@ -4248,6 +4260,1182 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16598403324584426"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.778578302712161"/>
+          <c:h val="0.7712809857101196"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'P3'!$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>one thread per row</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'P3'!$A$16:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'P3'!$B$16:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4999999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7B7E-4063-B436-FDD7B1D1EC97}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'P3'!$C$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>one group per row</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'P3'!$A$16:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'P3'!$C$16:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.6999999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3999999999999994E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.44E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1699999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0200000000000002E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7B7E-4063-B436-FDD7B1D1EC97}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1340869888"/>
+        <c:axId val="1340878624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1340869888"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="50000"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100"/>
+                  <a:t>number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                  <a:t> of rows</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1100"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1340878624"/>
+        <c:crossesAt val="1.0000000000000004E-5"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1340878624"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0000000000000002E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100"/>
+                  <a:t>execution time in s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1340869888"/>
+        <c:crossesAt val="100"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19570822397200349"/>
+          <c:y val="0.10705963837853603"/>
+          <c:w val="0.36090398075240593"/>
+          <c:h val="0.17866360454943131"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16598403324584426"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.778578302712161"/>
+          <c:h val="0.7712809857101196"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'P3'!$G$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>one thread per row</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'P3'!$A$16:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'P3'!$G$16:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.3E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9600000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5600000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.2700000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3450000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.588E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5019999999999999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F036-49EC-A25C-FE8763E5654D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'P3'!$H$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>one group per row</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'P3'!$A$16:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'P3'!$H$16:$H$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.3999999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.21E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5500000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5600000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.5600000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.4200000000000002E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F036-49EC-A25C-FE8763E5654D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1340869888"/>
+        <c:axId val="1340878624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1340869888"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="50000"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100"/>
+                  <a:t>number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                  <a:t> of rows</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1100"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1340878624"/>
+        <c:crossesAt val="1.0000000000000004E-5"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1340878624"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0000000000000002E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100"/>
+                  <a:t>execution time in s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1340869888"/>
+        <c:crossesAt val="100"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19570822397200349"/>
+          <c:y val="0.10705963837853603"/>
+          <c:w val="0.36090398075240593"/>
+          <c:h val="0.17866360454943131"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4448,6 +5636,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6513,6 +7781,1038 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7224,6 +9524,85 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>271462</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E4E298C-B2E1-4DD9-A0D8-636AD2058351}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{491BE27C-31DB-4A13-9492-634DE0A17533}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8620,10 +10999,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC7C974-8D29-467D-B540-E901A50BF91D}">
-  <dimension ref="A3:A10"/>
+  <dimension ref="A14:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8631,54 +11010,244 @@
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1">
-      <c r="A3">
-        <v>30</v>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
-        <f>A3*2</f>
-        <v>60</v>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5">
-        <f t="shared" ref="A5:A19" si="0">A4*2</f>
-        <v>120</v>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1">
+        <v>900</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2.3E-5</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3.6999999999999998E-5</v>
+      </c>
+      <c r="F16" s="1">
+        <v>900</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3.3E-4</v>
+      </c>
+      <c r="H16" s="2">
+        <v>6.3999999999999997E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>240</v>
+    <row r="17" spans="1:11">
+      <c r="A17" s="1">
+        <v>1600</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>5.5000000000000002E-5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1600</v>
+      </c>
+      <c r="G17" s="2">
+        <v>4.9600000000000002E-4</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1.21E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>480</v>
+    <row r="18" spans="1:11">
+      <c r="A18" s="1">
+        <v>2500</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2.3E-5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>6.7999999999999999E-5</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2500</v>
+      </c>
+      <c r="G18" s="2">
+        <v>6.5600000000000001E-4</v>
+      </c>
+      <c r="H18" s="2">
+        <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>960</v>
+    <row r="19" spans="1:11">
+      <c r="A19" s="1">
+        <v>3600</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3.4999999999999997E-5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>9.3999999999999994E-5</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3600</v>
+      </c>
+      <c r="G19" s="2">
+        <v>8.2700000000000004E-4</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2.5500000000000002E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>1920</v>
+    <row r="20" spans="1:11">
+      <c r="A20" s="1">
+        <v>6400</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1.44E-4</v>
+      </c>
+      <c r="F20" s="1">
+        <v>6400</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1.3450000000000001E-3</v>
+      </c>
+      <c r="H20" s="2">
+        <v>4.5600000000000003E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>3840</v>
-      </c>
+    <row r="21" spans="1:11">
+      <c r="A21" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B21" s="2">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2.1699999999999999E-4</v>
+      </c>
+      <c r="F21" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G21" s="2">
+        <v>2.588E-3</v>
+      </c>
+      <c r="H21" s="2">
+        <v>6.5600000000000001E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="1">
+        <v>14400</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2.9E-5</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3.0200000000000002E-4</v>
+      </c>
+      <c r="F22" s="1">
+        <v>14400</v>
+      </c>
+      <c r="G22" s="2">
+        <v>5.5019999999999999E-3</v>
+      </c>
+      <c r="H22" s="2">
+        <v>9.4200000000000002E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="E24" s="1"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="H32" s="2"/>
+    </row>
+    <row r="38" spans="5:7">
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="5:7">
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="5:7">
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="5:7">
+      <c r="E41" s="1"/>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="5:7">
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="5:7">
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="5:7">
+      <c r="E44" s="1"/>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="5:7">
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="5:7">
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="5:7">
+      <c r="E47" s="1"/>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="56" spans="7:7">
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="7:7">
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="7:7">
+      <c r="G58" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>